<commit_message>
TP#20088: CA cert tests
</commit_message>
<xml_diff>
--- a/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/CA Exp Dom.xlsx
+++ b/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/CA Exp Dom.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="186">
   <si>
     <t>CUSTOMER_REFERENCE</t>
   </si>
@@ -575,6 +575,15 @@
   </si>
   <si>
     <t>SaveLabel</t>
+  </si>
+  <si>
+    <t>RequestedShipment.ExpressFreightDetail</t>
+  </si>
+  <si>
+    <t>BookingConfirmationNumber</t>
+  </si>
+  <si>
+    <t>ShippersLoadAndCount</t>
   </si>
 </sst>
 </file>
@@ -2366,10 +2375,10 @@
   </sheetPr>
   <dimension ref="A1:JL641"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CH1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CK1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="CK3" sqref="CK3:CK14"/>
+      <selection pane="bottomLeft" activeCell="CM4" sqref="CM4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2707,8 +2716,12 @@
       <c r="CK1" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="CL1" s="20"/>
-      <c r="CM1" s="20"/>
+      <c r="CL1" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="CM1" s="20" t="s">
+        <v>183</v>
+      </c>
       <c r="CN1" s="20"/>
     </row>
     <row r="2" spans="1:92" s="9" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2973,8 +2986,12 @@
       <c r="CK2" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="CL2" s="7"/>
-      <c r="CM2" s="7"/>
+      <c r="CL2" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="CM2" s="7" t="s">
+        <v>185</v>
+      </c>
       <c r="CN2" s="7"/>
     </row>
     <row r="3" spans="1:92" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -3145,6 +3162,7 @@
       <c r="CK3" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="CM3" s="44"/>
     </row>
     <row r="4" spans="1:92" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="73" t="b">
@@ -3310,6 +3328,8 @@
       <c r="CK4" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="CL4" s="30"/>
+      <c r="CM4" s="30"/>
     </row>
     <row r="5" spans="1:92" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="73" t="b">
@@ -3489,8 +3509,10 @@
       <c r="CK5" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:92" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="CL5" s="30"/>
+      <c r="CM5" s="30"/>
+    </row>
+    <row r="6" spans="1:92" s="2" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="73" t="b">
         <v>0</v>
       </c>
@@ -3696,6 +3718,8 @@
       <c r="CK6" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="CL6" s="30"/>
+      <c r="CM6" s="30"/>
     </row>
     <row r="7" spans="1:92" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="73" t="b">
@@ -3885,6 +3909,12 @@
       <c r="CK7" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="CL7" s="44">
+        <v>1234567890</v>
+      </c>
+      <c r="CM7" s="44">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:92" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="73" t="b">
@@ -4074,6 +4104,8 @@
       <c r="CK8" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="CL8" s="35"/>
+      <c r="CM8" s="35"/>
     </row>
     <row r="9" spans="1:92" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="73" t="b">
@@ -4251,6 +4283,8 @@
       <c r="CK9" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="CL9" s="35"/>
+      <c r="CM9" s="35"/>
     </row>
     <row r="10" spans="1:92" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="73" t="b">
@@ -4416,6 +4450,8 @@
       <c r="CK10" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="CL10" s="35"/>
+      <c r="CM10" s="35"/>
     </row>
     <row r="11" spans="1:92" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="73" t="b">
@@ -4583,6 +4619,8 @@
       <c r="CK11" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="CL11" s="35"/>
+      <c r="CM11" s="35"/>
     </row>
     <row r="12" spans="1:92" s="2" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A12" s="73" t="b">
@@ -4772,6 +4810,8 @@
       <c r="CK12" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="CL12" s="61"/>
+      <c r="CM12" s="61"/>
     </row>
     <row r="13" spans="1:92" s="2" customFormat="1" ht="12.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" s="73" t="b">
@@ -4981,6 +5021,8 @@
       <c r="CK13" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="CL13" s="70"/>
+      <c r="CM13" s="70"/>
     </row>
     <row r="14" spans="1:92" s="2" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A14" s="73" t="b">
@@ -5154,6 +5196,8 @@
       <c r="CK14" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="CL14" s="52"/>
+      <c r="CM14" s="52"/>
     </row>
     <row r="15" spans="1:92" s="2" customFormat="1" ht="12.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>

</xml_diff>